<commit_message>
ROS-ToDo Formulierung zur Diskussion
</commit_message>
<xml_diff>
--- a/Zeitplanung/Zeitplan V2.xlsx
+++ b/Zeitplanung/Zeitplan V2.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
   <si>
     <t>KW 9</t>
   </si>
@@ -113,6 +113,9 @@
   </si>
   <si>
     <t>Aufbau Hardware</t>
+  </si>
+  <si>
+    <t>Grundsätzliche Auseinandersetzung mit ROS abgeschlossen</t>
   </si>
   <si>
     <t>Programmierung Fahrfunktion</t>
@@ -664,7 +667,7 @@
     <col min="2" max="2" style="15" width="44.71928571428572" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
     <col min="4" max="4" style="16" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="16" width="26.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="49.86214285714286" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="17" width="28.719285714285714" customWidth="1" bestFit="1"/>
     <col min="8" max="8" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
@@ -887,7 +890,9 @@
       </c>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+      <c r="E7" s="6" t="s">
+        <v>33</v>
+      </c>
       <c r="F7" s="6"/>
       <c r="G7" s="7"/>
       <c r="H7" s="6"/>
@@ -909,7 +914,7 @@
         <v>31</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -932,10 +937,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="2" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -958,10 +963,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -986,10 +991,10 @@
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
@@ -1020,7 +1025,7 @@
       <c r="E12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -1088,7 +1093,7 @@
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
       <c r="G15" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="H15" s="6"/>
       <c r="I15" s="6"/>

</xml_diff>

<commit_message>
tryoineg to resolve erros
</commit_message>
<xml_diff>
--- a/Zeitplanung/Zeitplan V2.xlsx
+++ b/Zeitplanung/Zeitplan V2.xlsx
@@ -14,7 +14,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
+  <si>
+    <t>KW8</t>
+  </si>
   <si>
     <t>KW 9</t>
   </si>
@@ -76,30 +79,45 @@
     <t>Recherche</t>
   </si>
   <si>
+    <t>Vergenauerung Zielsetzung</t>
+  </si>
+  <si>
+    <t>Hard und Software</t>
+  </si>
+  <si>
+    <t>Arbeitspaket 2</t>
+  </si>
+  <si>
+    <t>Anforderungen des Roboters festlegen</t>
+  </si>
+  <si>
+    <t>Aufgeschrieben</t>
+  </si>
+  <si>
+    <t>Arbeitspaket 3</t>
+  </si>
+  <si>
+    <t>Vergleich zu ähnlichen Konzepten</t>
+  </si>
+  <si>
+    <t>Information gesammelt</t>
+  </si>
+  <si>
     <t>x</t>
   </si>
   <si>
-    <t>Arbeitspaket 2</t>
-  </si>
-  <si>
-    <t>Anforderungen des Roboters festlegen</t>
-  </si>
-  <si>
-    <t>Arbeitspaket 3</t>
-  </si>
-  <si>
-    <t>Vergleich zu ähnlichen Konzepten</t>
-  </si>
-  <si>
-    <t>Information gesammelt</t>
-  </si>
-  <si>
     <t>Arbeitspaket 4</t>
   </si>
   <si>
     <t xml:space="preserve">grundsätzlich  Hardwareplanung abgeschlossen </t>
   </si>
   <si>
+    <t>Optionenliste</t>
+  </si>
+  <si>
+    <t>Diskussion über mögliche Hardware</t>
+  </si>
+  <si>
     <t>Marktrecherche abgeschlossen</t>
   </si>
   <si>
@@ -109,13 +127,17 @@
     <t>Strukturfestlegung Software</t>
   </si>
   <si>
+    <t>Grundsätzliche Auseinandersetzung
+grundsätzliche Auseinandersetzung</t>
+  </si>
+  <si>
     <t>Arbeitspaket 7</t>
   </si>
   <si>
     <t>Aufbau Hardware</t>
   </si>
   <si>
-    <t>Grundsätzliche Auseinandersetzung mit ROS abgeschlossen</t>
+    <t/>
   </si>
   <si>
     <t>Programmierung Fahrfunktion</t>
@@ -150,19 +172,13 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -310,41 +326,41 @@
     <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general" wrapText="1"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="3" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="5" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="4" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="6" applyBorder="1" fontId="3" applyFont="1" fillId="2" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="7" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="8" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="4" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
@@ -657,20 +673,20 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:T15"/>
+  <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="14" width="16.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="15" width="16.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="15" width="44.71928571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="16" width="20.433571428571426" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="16" width="49.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="17" width="28.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="16" width="19.14785714285714" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="16" width="28.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="16" width="39.14785714285715" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="16" width="49.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="17" width="28.719285714285714" customWidth="1" bestFit="1"/>
     <col min="9" max="9" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
     <col min="10" max="10" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
     <col min="11" max="11" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
@@ -683,12 +699,13 @@
     <col min="18" max="18" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
     <col min="19" max="19" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
     <col min="20" max="20" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
+    <col min="21" max="21" style="16" width="12.862142857142858" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="2" t="s">
+      <c r="B1" s="2"/>
+      <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
@@ -742,309 +759,337 @@
       <c r="T1" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="U1" s="2" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="20.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C2" s="5"/>
       <c r="D2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="6"/>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
-      <c r="M2" s="6"/>
-      <c r="N2" s="6"/>
-      <c r="O2" s="6"/>
-      <c r="P2" s="6"/>
-      <c r="Q2" s="6"/>
-      <c r="R2" s="6"/>
-      <c r="S2" s="6"/>
-      <c r="T2" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+      <c r="N2" s="5"/>
+      <c r="O2" s="5"/>
+      <c r="P2" s="5"/>
+      <c r="Q2" s="5"/>
+      <c r="R2" s="5"/>
+      <c r="S2" s="5"/>
+      <c r="T2" s="5"/>
+      <c r="U2" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="20.25">
       <c r="A3" s="2" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
+        <v>24</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6"/>
       <c r="E3" s="6"/>
-      <c r="F3" s="6"/>
-      <c r="G3" s="7"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="6"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="6"/>
-      <c r="T3" s="6"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="5"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="5"/>
+      <c r="L3" s="5"/>
+      <c r="M3" s="5"/>
+      <c r="N3" s="5"/>
+      <c r="O3" s="5"/>
+      <c r="P3" s="5"/>
+      <c r="Q3" s="5"/>
+      <c r="R3" s="5"/>
+      <c r="S3" s="5"/>
+      <c r="T3" s="5"/>
+      <c r="U3" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="20.25">
       <c r="A4" s="2" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6" t="s">
-        <v>25</v>
-      </c>
+        <v>27</v>
+      </c>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
       <c r="E4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" s="6"/>
-      <c r="G4" s="7"/>
-      <c r="H4" s="6"/>
-      <c r="I4" s="6"/>
-      <c r="J4" s="6"/>
-      <c r="K4" s="6"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="6"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="6"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="6"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="6"/>
-      <c r="T4" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="5"/>
+      <c r="J4" s="5"/>
+      <c r="K4" s="5"/>
+      <c r="L4" s="5"/>
+      <c r="M4" s="5"/>
+      <c r="N4" s="5"/>
+      <c r="O4" s="5"/>
+      <c r="P4" s="5"/>
+      <c r="Q4" s="5"/>
+      <c r="R4" s="5"/>
+      <c r="S4" s="5"/>
+      <c r="T4" s="5"/>
+      <c r="U4" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="20.25">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="5"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
-      <c r="J5" s="6"/>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="6"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="6"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="6"/>
-      <c r="T5" s="6"/>
+        <v>31</v>
+      </c>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G5" s="6"/>
+      <c r="H5" s="9"/>
+      <c r="I5" s="5"/>
+      <c r="J5" s="5"/>
+      <c r="K5" s="5"/>
+      <c r="L5" s="5"/>
+      <c r="M5" s="5"/>
+      <c r="N5" s="5"/>
+      <c r="O5" s="5"/>
+      <c r="P5" s="5"/>
+      <c r="Q5" s="5"/>
+      <c r="R5" s="5"/>
+      <c r="S5" s="5"/>
+      <c r="T5" s="5"/>
+      <c r="U5" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="20.25">
       <c r="A6" s="2" t="s">
-        <v>29</v>
+        <v>35</v>
       </c>
       <c r="B6" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="5"/>
-      <c r="I6" s="5"/>
-      <c r="J6" s="5"/>
+        <v>36</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="7"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
       <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
+      <c r="L6" s="5"/>
+      <c r="M6" s="5"/>
+      <c r="N6" s="5"/>
+      <c r="O6" s="5"/>
+      <c r="P6" s="5"/>
+      <c r="Q6" s="5"/>
+      <c r="R6" s="5"/>
+      <c r="S6" s="5"/>
+      <c r="T6" s="5"/>
+      <c r="U6" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="20.25">
       <c r="A7" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B7" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F7" s="6"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="12" t="s">
+        <v>40</v>
+      </c>
+      <c r="G7" s="5"/>
+      <c r="H7" s="7"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="5"/>
-      <c r="K7" s="5"/>
-      <c r="L7" s="5"/>
+      <c r="K7" s="6"/>
+      <c r="L7" s="6"/>
       <c r="M7" s="6"/>
-      <c r="N7" s="6"/>
-      <c r="O7" s="6"/>
-      <c r="P7" s="6"/>
-      <c r="Q7" s="6"/>
-      <c r="R7" s="6"/>
-      <c r="S7" s="6"/>
-      <c r="T7" s="6"/>
+      <c r="N7" s="5"/>
+      <c r="O7" s="5"/>
+      <c r="P7" s="5"/>
+      <c r="Q7" s="5"/>
+      <c r="R7" s="5"/>
+      <c r="S7" s="5"/>
+      <c r="T7" s="5"/>
+      <c r="U7" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="20.25">
       <c r="A8" s="2" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
-      <c r="K8" s="6"/>
+        <v>41</v>
+      </c>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="7"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+      <c r="K8" s="5"/>
       <c r="L8" s="5"/>
-      <c r="M8" s="5"/>
-      <c r="N8" s="5"/>
+      <c r="M8" s="6"/>
+      <c r="N8" s="6"/>
       <c r="O8" s="6"/>
-      <c r="P8" s="6"/>
-      <c r="Q8" s="6"/>
-      <c r="R8" s="6"/>
-      <c r="S8" s="6"/>
-      <c r="T8" s="6"/>
+      <c r="P8" s="5"/>
+      <c r="Q8" s="5"/>
+      <c r="R8" s="5"/>
+      <c r="S8" s="5"/>
+      <c r="T8" s="5"/>
+      <c r="U8" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="20.25">
       <c r="A9" s="2" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
+        <v>43</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="7"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
       <c r="L9" s="5"/>
-      <c r="M9" s="5"/>
-      <c r="N9" s="5"/>
-      <c r="O9" s="5"/>
-      <c r="P9" s="5"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
       <c r="Q9" s="6"/>
-      <c r="R9" s="6"/>
-      <c r="S9" s="6"/>
-      <c r="T9" s="6"/>
+      <c r="R9" s="5"/>
+      <c r="S9" s="5"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="20.25">
       <c r="A10" s="2" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B10" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="6"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="6"/>
-      <c r="M10" s="6"/>
-      <c r="N10" s="6"/>
-      <c r="O10" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="P10" s="5"/>
-      <c r="Q10" s="5"/>
-      <c r="R10" s="5"/>
+        <v>45</v>
+      </c>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="7"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+      <c r="K10" s="5"/>
+      <c r="L10" s="5"/>
+      <c r="M10" s="5"/>
+      <c r="N10" s="5"/>
+      <c r="O10" s="5"/>
+      <c r="P10" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q10" s="6"/>
+      <c r="R10" s="6"/>
       <c r="S10" s="6"/>
-      <c r="T10" s="6"/>
+      <c r="T10" s="5"/>
+      <c r="U10" s="5"/>
     </row>
     <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="20.25">
       <c r="A11" s="2" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B11" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="6"/>
-      <c r="E11" s="6"/>
-      <c r="F11" s="6"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
-      <c r="K11" s="6"/>
-      <c r="L11" s="6"/>
-      <c r="M11" s="6"/>
-      <c r="N11" s="6"/>
-      <c r="O11" s="6"/>
-      <c r="P11" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="Q11" s="6"/>
-      <c r="R11" s="6"/>
+        <v>47</v>
+      </c>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+      <c r="K11" s="5"/>
+      <c r="L11" s="5"/>
+      <c r="M11" s="5"/>
+      <c r="N11" s="5"/>
+      <c r="O11" s="5"/>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="R11" s="5"/>
       <c r="S11" s="5"/>
-      <c r="T11" s="5"/>
+      <c r="T11" s="6"/>
+      <c r="U11" s="6"/>
     </row>
     <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="33" customFormat="1" s="1">
-      <c r="A12" s="3"/>
-      <c r="B12" s="3"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
       <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="3"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="13" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="2"/>
+      <c r="L12" s="2"/>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+      <c r="O12" s="2"/>
+      <c r="P12" s="2"/>
+      <c r="Q12" s="2"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="2"/>
+      <c r="T12" s="2"/>
+      <c r="U12" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="3"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
@@ -1062,11 +1107,12 @@
       <c r="R13" s="2"/>
       <c r="S13" s="2"/>
       <c r="T13" s="2"/>
+      <c r="U13" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="19.5" customFormat="1" s="1">
       <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="3"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
@@ -1084,30 +1130,32 @@
       <c r="R14" s="2"/>
       <c r="S14" s="2"/>
       <c r="T14" s="2"/>
+      <c r="U14" s="2"/>
     </row>
     <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="19.5">
       <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="6"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="6"/>
-      <c r="F15" s="6"/>
-      <c r="G15" s="13" t="s">
-        <v>42</v>
-      </c>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="6"/>
-      <c r="L15" s="6"/>
-      <c r="M15" s="6"/>
-      <c r="N15" s="6"/>
-      <c r="O15" s="6"/>
-      <c r="P15" s="6"/>
-      <c r="Q15" s="6"/>
-      <c r="R15" s="6"/>
-      <c r="S15" s="6"/>
-      <c r="T15" s="6"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="5"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="5"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
+      <c r="N15" s="5"/>
+      <c r="O15" s="5"/>
+      <c r="P15" s="5"/>
+      <c r="Q15" s="5"/>
+      <c r="R15" s="5"/>
+      <c r="S15" s="5"/>
+      <c r="T15" s="5"/>
+      <c r="U15" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>